<commit_message>
Data driven Testing for LoginTest
</commit_message>
<xml_diff>
--- a/src/main/java/data.xlsx
+++ b/src/main/java/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11370" windowHeight="2490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="6120"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>tutorial</t>
   </si>
 </sst>
 </file>
@@ -365,14 +362,14 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>

</xml_diff>